<commit_message>
PS table for Trigger review updated with BParking seeds enabled for main + specific block
</commit_message>
<xml_diff>
--- a/development/L1Menu_Collisions2022_v0_1_2/PrescaleTable/NovemberTriggerReview_dedicatedPStableForRateStudy_L1Menu_Collisions2022_v0_1_2.xlsx
+++ b/development/L1Menu_Collisions2022_v0_1_2/PrescaleTable/NovemberTriggerReview_dedicatedPStableForRateStudy_L1Menu_Collisions2022_v0_1_2.xlsx
@@ -1422,7 +1422,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
@@ -8538,7 +8541,7 @@
         <v>0.0</v>
       </c>
       <c r="E174" s="3">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="F174" s="3">
         <v>0.0</v>
@@ -8547,7 +8550,7 @@
         <v>0.0</v>
       </c>
       <c r="H174" s="3">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="I174" s="3">
         <v>0.0</v>
@@ -8559,7 +8562,7 @@
         <v>0.0</v>
       </c>
       <c r="L174" s="3">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="M174" s="3">
         <v>0.0</v>

</xml_diff>